<commit_message>
MapPrototype3 - Minor fix
Small update to prevent loophole
</commit_message>
<xml_diff>
--- a/Assets/MapPrototypeDesign.xlsx
+++ b/Assets/MapPrototypeDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TL\Personal\Projects_Self\2023gamejamcssa\2023gamejamcssa\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C722E3-B64F-4301-AA2D-EAA7A86AC589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46065E97-C2AC-44AB-B354-8A6A6B8F0E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{F6FA76B0-B0FB-44AE-A37A-4F9737DD96F1}"/>
+    <workbookView xWindow="9360" yWindow="1908" windowWidth="7500" windowHeight="6000" activeTab="2" xr2:uid="{F6FA76B0-B0FB-44AE-A37A-4F9737DD96F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1055,7 +1055,7 @@
   <dimension ref="A1:AW32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="46" zoomScaleNormal="46" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2821,8 +2821,8 @@
       <c r="V18" s="68">
         <v>909</v>
       </c>
-      <c r="W18" s="81">
-        <v>11</v>
+      <c r="W18" s="68">
+        <v>909</v>
       </c>
       <c r="X18" s="18">
         <v>0</v>
@@ -4120,7 +4120,7 @@
   <dimension ref="A1:AW32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="46" zoomScaleNormal="46" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.6640625" defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5176,8 +5176,8 @@
       <c r="V18" s="68">
         <v>909</v>
       </c>
-      <c r="W18" s="22">
-        <v>11</v>
+      <c r="W18" s="68">
+        <v>909</v>
       </c>
       <c r="X18" s="18"/>
       <c r="Y18" s="18"/>
@@ -5899,7 +5899,7 @@
   <dimension ref="A1:AW32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="46" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7729,8 +7729,8 @@
       <c r="V18" s="33">
         <v>909</v>
       </c>
-      <c r="W18" s="22">
-        <v>11</v>
+      <c r="W18" s="33">
+        <v>909</v>
       </c>
       <c r="X18" s="17">
         <v>99</v>

</xml_diff>